<commit_message>
units corrections for parts in M40, M148, and prewetter
</commit_message>
<xml_diff>
--- a/OpsAndMats/Model148.xlsx
+++ b/OpsAndMats/Model148.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclark.LABTESTING\Documents\ERP Notes\Phase2_BOM\OpsAndMats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFB31DB-1979-4657-A470-4DD30505CA0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Operations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="193">
   <si>
     <t>Item</t>
   </si>
@@ -170,246 +164,246 @@
     <t>8026417-2</t>
   </si>
   <si>
+    <t>8026391</t>
+  </si>
+  <si>
+    <t>8034957</t>
+  </si>
+  <si>
+    <t>8034957-G</t>
+  </si>
+  <si>
+    <t>8034957-H</t>
+  </si>
+  <si>
+    <t>8034957-A</t>
+  </si>
+  <si>
+    <t>8034957-E</t>
+  </si>
+  <si>
+    <t>8034957-F</t>
+  </si>
+  <si>
+    <t>8034957-B</t>
+  </si>
+  <si>
+    <t>8034957-C</t>
+  </si>
+  <si>
+    <t>8035009-X</t>
+  </si>
+  <si>
+    <t>8035009-A</t>
+  </si>
+  <si>
+    <t>8035009-B</t>
+  </si>
+  <si>
+    <t>8035009-1</t>
+  </si>
+  <si>
+    <t>8035009-2</t>
+  </si>
+  <si>
+    <t>8035009-3</t>
+  </si>
+  <si>
+    <t>8035009-4</t>
+  </si>
+  <si>
+    <t>MODEL 148AC INSTRUMENT STAND WITH MAC-F…</t>
+  </si>
+  <si>
+    <t>SHELF FOR MODEL 148AC INSTRUMENT CABINE…</t>
+  </si>
+  <si>
+    <t>EXTENSION FOOT ASSEMBLY FOR MOD 76E TES…</t>
+  </si>
+  <si>
+    <t>Leg Lagging Plate</t>
+  </si>
+  <si>
+    <t>WELD ASSEMBLY FOR MODEL 148AC INSTRUMEN…</t>
+  </si>
+  <si>
+    <t>MOUNTING PLATE WELD ASSEMBLY FOR MAC-FD…</t>
+  </si>
+  <si>
+    <t>ASY010</t>
+  </si>
+  <si>
+    <t>FAB010</t>
+  </si>
+  <si>
+    <t>FIN020</t>
+  </si>
+  <si>
+    <t>FAB070</t>
+  </si>
+  <si>
+    <t>EXT010</t>
+  </si>
+  <si>
+    <t>Assembly, System</t>
+  </si>
+  <si>
+    <t>Fabrication, Saw</t>
+  </si>
+  <si>
+    <t>Finishing, Paint</t>
+  </si>
+  <si>
+    <t>Fabrication, Welding</t>
+  </si>
+  <si>
+    <t>External Operations</t>
+  </si>
+  <si>
+    <t>1421705</t>
+  </si>
+  <si>
+    <t>1606101</t>
+  </si>
+  <si>
+    <t>1506101</t>
+  </si>
+  <si>
+    <t>7181005</t>
+  </si>
+  <si>
+    <t>7181006</t>
+  </si>
+  <si>
+    <t>7181004</t>
+  </si>
+  <si>
+    <t>7181007</t>
+  </si>
+  <si>
+    <t>2292008</t>
+  </si>
+  <si>
+    <t>2152002</t>
+  </si>
+  <si>
+    <t>9561031-A</t>
+  </si>
+  <si>
+    <t>9735003</t>
+  </si>
+  <si>
+    <t>9710001</t>
+  </si>
+  <si>
+    <t>2507201</t>
+  </si>
+  <si>
+    <t>2577201</t>
+  </si>
+  <si>
+    <t>2402006</t>
+  </si>
+  <si>
+    <t>9691050</t>
+  </si>
+  <si>
+    <t>9812001</t>
+  </si>
+  <si>
     <t>8025044-9</t>
   </si>
   <si>
-    <t>8026391</t>
-  </si>
-  <si>
-    <t>8034957</t>
-  </si>
-  <si>
-    <t>8034957-G</t>
-  </si>
-  <si>
-    <t>8034957-H</t>
-  </si>
-  <si>
-    <t>8034957-A</t>
-  </si>
-  <si>
-    <t>8034957-E</t>
-  </si>
-  <si>
-    <t>8034957-F</t>
-  </si>
-  <si>
-    <t>8034957-B</t>
-  </si>
-  <si>
-    <t>8034957-C</t>
-  </si>
-  <si>
-    <t>8035009-X</t>
-  </si>
-  <si>
-    <t>8035009-A</t>
-  </si>
-  <si>
-    <t>8035009-B</t>
-  </si>
-  <si>
-    <t>8035009-1</t>
-  </si>
-  <si>
-    <t>8035009-2</t>
-  </si>
-  <si>
-    <t>8035009-3</t>
-  </si>
-  <si>
-    <t>8035009-4</t>
-  </si>
-  <si>
-    <t>MODEL 148AC INSTRUMENT STAND WITH MAC-F…</t>
-  </si>
-  <si>
-    <t>SHELF FOR MODEL 148AC INSTRUMENT CABINE…</t>
-  </si>
-  <si>
-    <t>EXTENSION FOOT ASSEMBLY FOR MOD 76E TES…</t>
+    <t>2034701</t>
+  </si>
+  <si>
+    <t>9030240-3</t>
+  </si>
+  <si>
+    <t>6960011</t>
+  </si>
+  <si>
+    <t>9816001</t>
+  </si>
+  <si>
+    <t>3130003</t>
+  </si>
+  <si>
+    <t>9018204-2</t>
+  </si>
+  <si>
+    <t>9011243</t>
+  </si>
+  <si>
+    <t>9014122-4</t>
+  </si>
+  <si>
+    <t>SHCS, 10-32, 5/8, St. Stl.</t>
+  </si>
+  <si>
+    <t>Washer, Lock, Ext. Tooth, #10, St. Stl.</t>
+  </si>
+  <si>
+    <t>Washer, Standard, #10, St. Stl.</t>
+  </si>
+  <si>
+    <t>Wall Mount LCD Arm, LX, Sit-Stand</t>
+  </si>
+  <si>
+    <t>Wall Mount Keyboard Arm, LX</t>
+  </si>
+  <si>
+    <t>Wall Track, 26"</t>
+  </si>
+  <si>
+    <t>Wall Mount Mounting Bracket</t>
+  </si>
+  <si>
+    <t>M.Scr, 82°FH, ¼-20, 1, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>Nut, Self Clinching, ¼-20, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>ABS Plastic, 1/32" thk., 1/2" wide.</t>
+  </si>
+  <si>
+    <t>Light Duty Mounting Tape, 1/2" wd.</t>
+  </si>
+  <si>
+    <t>Thread Locker, Low Torque, Purple</t>
+  </si>
+  <si>
+    <t>Washer, Standard, ¼, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>Washer, Split Lock, Med, ¼, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>HHCS, ¼-20, 3/4, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>Sheet, MDF, 1/2" thk.</t>
+  </si>
+  <si>
+    <t>Paint, Polane B, Circuit Blue</t>
   </si>
   <si>
     <t>Threaded Rod, Zinc Plated</t>
   </si>
   <si>
-    <t>Leg Lagging Plate</t>
-  </si>
-  <si>
-    <t>WELD ASSEMBLY FOR MODEL 148AC INSTRUMEN…</t>
-  </si>
-  <si>
-    <t>MOUNTING PLATE WELD ASSEMBLY FOR MAC-FD…</t>
-  </si>
-  <si>
-    <t>ASY010</t>
-  </si>
-  <si>
-    <t>FAB010</t>
-  </si>
-  <si>
-    <t>FIN020</t>
-  </si>
-  <si>
-    <t>EXT010</t>
-  </si>
-  <si>
-    <t>FAB070</t>
-  </si>
-  <si>
-    <t>Assembly, System</t>
-  </si>
-  <si>
-    <t>Fabrication, Saw</t>
-  </si>
-  <si>
-    <t>Finishing, Paint</t>
-  </si>
-  <si>
-    <t>External Operations</t>
-  </si>
-  <si>
-    <t>Fabrication, Welding</t>
-  </si>
-  <si>
-    <t>1421705</t>
-  </si>
-  <si>
-    <t>1606101</t>
-  </si>
-  <si>
-    <t>1506101</t>
-  </si>
-  <si>
-    <t>7181005</t>
-  </si>
-  <si>
-    <t>7181006</t>
-  </si>
-  <si>
-    <t>7181004</t>
-  </si>
-  <si>
-    <t>7181007</t>
-  </si>
-  <si>
-    <t>2292008</t>
-  </si>
-  <si>
-    <t>2152002</t>
-  </si>
-  <si>
-    <t>9561031-A</t>
-  </si>
-  <si>
-    <t>9735003</t>
-  </si>
-  <si>
-    <t>9710001</t>
-  </si>
-  <si>
-    <t>2507201</t>
-  </si>
-  <si>
-    <t>2577201</t>
-  </si>
-  <si>
-    <t>2402006</t>
-  </si>
-  <si>
-    <t>9691050</t>
-  </si>
-  <si>
-    <t>9812001</t>
-  </si>
-  <si>
-    <t>2034701</t>
-  </si>
-  <si>
-    <t>9816001</t>
-  </si>
-  <si>
-    <t>9030240-3</t>
-  </si>
-  <si>
-    <t>6960011</t>
-  </si>
-  <si>
-    <t>3130003</t>
-  </si>
-  <si>
-    <t>9018204-2</t>
-  </si>
-  <si>
-    <t>9011243</t>
-  </si>
-  <si>
-    <t>9014122-4</t>
-  </si>
-  <si>
-    <t>SHCS, 10-32, 5/8, St. Stl.</t>
-  </si>
-  <si>
-    <t>Washer, Lock, Ext. Tooth, #10, St. Stl.</t>
-  </si>
-  <si>
-    <t>Washer, Standard, #10, St. Stl.</t>
-  </si>
-  <si>
-    <t>Wall Mount LCD Arm, LX, Sit-Stand</t>
-  </si>
-  <si>
-    <t>Wall Mount Keyboard Arm, LX</t>
-  </si>
-  <si>
-    <t>Wall Track, 26"</t>
-  </si>
-  <si>
-    <t>Wall Mount Mounting Bracket</t>
-  </si>
-  <si>
-    <t>M.Scr, 82°FH, ¼-20, 1, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>Nut, Self Clinching, ¼-20, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>ABS Plastic, 1/32" thk., 1/2" wide.</t>
-  </si>
-  <si>
-    <t>Light Duty Mounting Tape, 1/2" wd.</t>
-  </si>
-  <si>
-    <t>Thread Locker, Low Torque, Purple</t>
-  </si>
-  <si>
-    <t>Washer, Standard, ¼, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>Washer, Split Lock, Med, ¼, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>HHCS, ¼-20, 3/4, Pl. Stl.</t>
-  </si>
-  <si>
-    <t>Sheet, MDF, 1/2" thk.</t>
-  </si>
-  <si>
-    <t>Paint, Polane B, Circuit Blue</t>
-  </si>
-  <si>
-    <t>Nut, ASF full, 1-8, Pl. Stl.</t>
+    <t>Hex Nut, full, 1-8, Pl. Stl.</t>
+  </si>
+  <si>
+    <t>5/16 x 2-1/2" CRS Bar</t>
+  </si>
+  <si>
+    <t>swivel pad with 1"-8 thd.</t>
   </si>
   <si>
     <t>Nickel Plating, Electroless</t>
   </si>
   <si>
-    <t>5/16 x 2-1/2" CRS Bar</t>
-  </si>
-  <si>
-    <t>swivel pad with 1"-8 thd.</t>
-  </si>
-  <si>
     <t>1"-8 heavy square nut, unplated</t>
   </si>
   <si>
@@ -428,13 +422,13 @@
     <t>EA</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>SF</t>
   </si>
   <si>
     <t>g</t>
-  </si>
-  <si>
-    <t>IN</t>
   </si>
   <si>
     <t>Use Fixed Schedule</t>
@@ -605,8 +599,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,14 +663,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -723,7 +709,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,27 +741,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,24 +775,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1000,16 +950,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AQ71"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1140,27 +1088,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1223,27 +1171,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
         <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -1306,27 +1254,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
         <v>47</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4">
         <v>3</v>
@@ -1389,27 +1337,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -1472,27 +1420,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -1555,27 +1503,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K7">
         <v>6</v>
@@ -1638,27 +1586,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K8">
         <v>7</v>
@@ -1721,27 +1669,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K9">
         <v>8</v>
@@ -1804,27 +1752,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K10">
         <v>9</v>
@@ -1887,27 +1835,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K11">
         <v>10</v>
@@ -1970,27 +1918,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12">
         <v>11</v>
@@ -2053,27 +2001,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K13">
         <v>12</v>
@@ -2136,27 +2084,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K14">
         <v>13</v>
@@ -2219,27 +2167,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K15">
         <v>14</v>
@@ -2302,27 +2250,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K16">
         <v>15</v>
@@ -2385,27 +2333,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43">
       <c r="A17" t="s">
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K17">
         <v>16</v>
@@ -2468,27 +2416,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18" t="s">
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K18">
         <v>17</v>
@@ -2503,13 +2451,13 @@
         <v>8</v>
       </c>
       <c r="S18">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="T18" t="s">
         <v>133</v>
       </c>
       <c r="U18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -2551,27 +2499,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K19">
         <v>18</v>
@@ -2586,13 +2534,13 @@
         <v>8</v>
       </c>
       <c r="S19">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="T19" t="s">
         <v>133</v>
       </c>
       <c r="U19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -2634,27 +2582,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K20">
         <v>19</v>
@@ -2669,7 +2617,7 @@
         <v>8</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T20" t="s">
         <v>133</v>
@@ -2717,27 +2665,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K21">
         <v>20</v>
@@ -2752,7 +2700,7 @@
         <v>8</v>
       </c>
       <c r="S21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T21" t="s">
         <v>133</v>
@@ -2800,27 +2748,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22" t="s">
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K22">
         <v>21</v>
@@ -2883,27 +2831,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23" t="s">
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K23">
         <v>22</v>
@@ -2966,33 +2914,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24">
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -3001,7 +2949,7 @@
         <v>8</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T24" t="s">
         <v>133</v>
@@ -3049,27 +2997,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
         <v>43</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -3132,27 +3080,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
         <v>43</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3215,33 +3163,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27">
         <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="J27" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -3298,33 +3246,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28" t="s">
         <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28">
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -3381,33 +3329,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29">
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -3464,33 +3412,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30" t="s">
         <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -3499,7 +3447,7 @@
         <v>8</v>
       </c>
       <c r="S30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T30" t="s">
         <v>133</v>
@@ -3547,33 +3495,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31" t="s">
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -3582,7 +3530,7 @@
         <v>8</v>
       </c>
       <c r="S31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T31" t="s">
         <v>133</v>
@@ -3630,33 +3578,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32" t="s">
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -3713,33 +3661,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I33" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="J33" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -3748,13 +3696,13 @@
         <v>8</v>
       </c>
       <c r="S33">
-        <v>1.25</v>
+        <v>3</v>
       </c>
       <c r="T33" t="s">
         <v>133</v>
       </c>
       <c r="U33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -3796,27 +3744,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34" t="s">
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -3831,7 +3779,7 @@
         <v>8</v>
       </c>
       <c r="S34">
-        <v>25</v>
+        <v>1.25</v>
       </c>
       <c r="T34" t="s">
         <v>133</v>
@@ -3879,15 +3827,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G35" t="s">
         <v>73</v>
@@ -3896,10 +3844,10 @@
         <v>78</v>
       </c>
       <c r="I35" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="J35" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -3914,13 +3862,13 @@
         <v>8</v>
       </c>
       <c r="S35">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T35" t="s">
         <v>133</v>
       </c>
       <c r="U35" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V35">
         <v>0</v>
@@ -3962,33 +3910,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36" t="s">
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36">
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -3997,7 +3945,7 @@
         <v>8</v>
       </c>
       <c r="S36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T36" t="s">
         <v>133</v>
@@ -4045,33 +3993,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37" t="s">
         <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37">
         <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I37" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="J37" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="K37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -4080,7 +4028,7 @@
         <v>8</v>
       </c>
       <c r="S37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T37" t="s">
         <v>133</v>
@@ -4128,33 +4076,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E38">
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I38" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="J38" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M38">
         <v>0</v>
@@ -4163,13 +4111,13 @@
         <v>8</v>
       </c>
       <c r="S38">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="T38" t="s">
         <v>133</v>
       </c>
       <c r="U38" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -4211,27 +4159,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E39">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" t="s">
         <v>77</v>
       </c>
-      <c r="H39" t="s">
-        <v>82</v>
-      </c>
       <c r="I39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -4246,13 +4194,13 @@
         <v>8</v>
       </c>
       <c r="S39">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="T39" t="s">
         <v>133</v>
       </c>
       <c r="U39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V39">
         <v>0</v>
@@ -4294,27 +4242,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43">
       <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40">
         <v>50</v>
       </c>
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40">
-        <v>60</v>
-      </c>
       <c r="G40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I40" t="s">
         <v>101</v>
       </c>
       <c r="J40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -4377,27 +4325,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E41">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I41" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="J41" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -4460,33 +4408,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E42">
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H42" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42">
         <v>0</v>
@@ -4543,33 +4491,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43">
         <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H43" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I43" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M43">
         <v>0</v>
@@ -4578,7 +4526,7 @@
         <v>8</v>
       </c>
       <c r="S43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T43" t="s">
         <v>133</v>
@@ -4626,33 +4574,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E44">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I44" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="J44" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="K44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -4661,13 +4609,13 @@
         <v>8</v>
       </c>
       <c r="S44">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="T44" t="s">
         <v>133</v>
       </c>
       <c r="U44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V44">
         <v>0</v>
@@ -4709,27 +4657,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E45">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H45" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I45" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="J45" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -4744,13 +4692,13 @@
         <v>8</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T45" t="s">
         <v>133</v>
       </c>
       <c r="U45" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -4792,33 +4740,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E46">
         <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M46">
         <v>0</v>
@@ -4827,7 +4775,7 @@
         <v>8</v>
       </c>
       <c r="S46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T46" t="s">
         <v>133</v>
@@ -4875,33 +4823,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E47">
         <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -4910,7 +4858,7 @@
         <v>8</v>
       </c>
       <c r="S47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T47" t="s">
         <v>133</v>
@@ -4958,33 +4906,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E48">
         <v>10</v>
       </c>
       <c r="G48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -5041,33 +4989,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E49">
         <v>10</v>
       </c>
       <c r="G49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I49" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="J49" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="K49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M49">
         <v>0</v>
@@ -5076,7 +5024,7 @@
         <v>8</v>
       </c>
       <c r="S49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T49" t="s">
         <v>133</v>
@@ -5124,33 +5072,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E50">
         <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I50" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="J50" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M50">
         <v>0</v>
@@ -5159,7 +5107,7 @@
         <v>8</v>
       </c>
       <c r="S50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T50" t="s">
         <v>133</v>
@@ -5207,33 +5155,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E51">
         <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H51" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I51" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J51" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -5242,7 +5190,7 @@
         <v>8</v>
       </c>
       <c r="S51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T51" t="s">
         <v>133</v>
@@ -5290,33 +5238,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E52">
         <v>10</v>
       </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H52" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I52" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J52" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -5373,33 +5321,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E53">
         <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I53" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="J53" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="K53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -5456,12 +5404,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E54">
         <v>10</v>
@@ -5473,16 +5421,16 @@
         <v>79</v>
       </c>
       <c r="I54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -5491,13 +5439,13 @@
         <v>8</v>
       </c>
       <c r="S54">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="T54" t="s">
         <v>133</v>
       </c>
       <c r="U54" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -5539,24 +5487,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E55">
         <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H55" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J55" t="s">
         <v>130</v>
@@ -5580,7 +5528,7 @@
         <v>133</v>
       </c>
       <c r="U55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -5622,24 +5570,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E56">
         <v>10</v>
       </c>
       <c r="G56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H56" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J56" t="s">
         <v>130</v>
@@ -5663,7 +5611,7 @@
         <v>133</v>
       </c>
       <c r="U56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V56">
         <v>0</v>
@@ -5705,24 +5653,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E57">
         <v>10</v>
       </c>
       <c r="G57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J57" t="s">
         <v>130</v>
@@ -5740,13 +5688,13 @@
         <v>8</v>
       </c>
       <c r="S57">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="T57" t="s">
         <v>133</v>
       </c>
       <c r="U57" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V57">
         <v>0</v>
@@ -5788,24 +5736,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E58">
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H58" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J58" t="s">
         <v>130</v>
@@ -5823,13 +5771,13 @@
         <v>8</v>
       </c>
       <c r="S58">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="T58" t="s">
         <v>133</v>
       </c>
       <c r="U58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V58">
         <v>0</v>
@@ -5871,27 +5819,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E59">
         <v>10</v>
       </c>
       <c r="G59" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" t="s">
         <v>77</v>
       </c>
-      <c r="H59" t="s">
-        <v>82</v>
-      </c>
       <c r="I59" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="J59" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -5906,13 +5854,13 @@
         <v>8</v>
       </c>
       <c r="S59">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="T59" t="s">
         <v>133</v>
       </c>
       <c r="U59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -5954,33 +5902,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E60">
         <v>10</v>
       </c>
       <c r="G60" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M60">
         <v>0</v>
@@ -6037,12 +5985,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E61">
         <v>10</v>
@@ -6054,16 +6002,16 @@
         <v>79</v>
       </c>
       <c r="I61" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="J61" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="K61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M61">
         <v>0</v>
@@ -6072,13 +6020,13 @@
         <v>8</v>
       </c>
       <c r="S61">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T61" t="s">
         <v>133</v>
       </c>
       <c r="U61" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -6120,27 +6068,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E62">
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H62" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -6155,13 +6103,13 @@
         <v>8</v>
       </c>
       <c r="S62">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="T62" t="s">
         <v>133</v>
       </c>
       <c r="U62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V62">
         <v>0</v>
@@ -6203,27 +6151,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E63">
         <v>10</v>
       </c>
       <c r="G63" t="s">
+        <v>72</v>
+      </c>
+      <c r="H63" t="s">
         <v>77</v>
       </c>
-      <c r="H63" t="s">
-        <v>82</v>
-      </c>
       <c r="I63" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="J63" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -6238,13 +6186,13 @@
         <v>8</v>
       </c>
       <c r="S63">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T63" t="s">
         <v>133</v>
       </c>
       <c r="U63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="V63">
         <v>0</v>
@@ -6286,27 +6234,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E64">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I64" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="J64" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -6321,13 +6269,13 @@
         <v>8</v>
       </c>
       <c r="S64">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="T64" t="s">
         <v>133</v>
       </c>
       <c r="U64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V64">
         <v>0</v>
@@ -6369,27 +6317,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E65">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G65" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H65" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I65" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="J65" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -6404,13 +6352,13 @@
         <v>8</v>
       </c>
       <c r="S65">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T65" t="s">
         <v>133</v>
       </c>
       <c r="U65" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V65">
         <v>0</v>
@@ -6452,27 +6400,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E66">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I66" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="J66" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -6487,13 +6435,13 @@
         <v>8</v>
       </c>
       <c r="S66">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="T66" t="s">
         <v>133</v>
       </c>
       <c r="U66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V66">
         <v>0</v>
@@ -6535,27 +6483,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E67">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G67" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H67" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I67" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="J67" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -6570,13 +6518,13 @@
         <v>8</v>
       </c>
       <c r="S67">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T67" t="s">
         <v>133</v>
       </c>
       <c r="U67" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V67">
         <v>0</v>
@@ -6618,27 +6566,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E68">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I68" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="J68" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="K68">
         <v>1</v>
@@ -6653,13 +6601,13 @@
         <v>8</v>
       </c>
       <c r="S68">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="T68" t="s">
         <v>133</v>
       </c>
       <c r="U68" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V68">
         <v>0</v>
@@ -6701,27 +6649,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E69">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G69" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H69" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I69" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="J69" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -6736,13 +6684,13 @@
         <v>8</v>
       </c>
       <c r="S69">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T69" t="s">
         <v>133</v>
       </c>
       <c r="U69" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V69">
         <v>0</v>
@@ -6784,27 +6732,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E70">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I70" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="J70" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -6819,13 +6767,13 @@
         <v>8</v>
       </c>
       <c r="S70">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="T70" t="s">
         <v>133</v>
       </c>
       <c r="U70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V70">
         <v>0</v>
@@ -6864,6 +6812,89 @@
         <v>0</v>
       </c>
       <c r="AQ70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:43">
+      <c r="A71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71">
+        <v>30</v>
+      </c>
+      <c r="G71" t="s">
+        <v>73</v>
+      </c>
+      <c r="H71" t="s">
+        <v>78</v>
+      </c>
+      <c r="I71" t="s">
+        <v>97</v>
+      </c>
+      <c r="J71" t="s">
+        <v>123</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="R71" t="s">
+        <v>8</v>
+      </c>
+      <c r="S71">
+        <v>25</v>
+      </c>
+      <c r="T71" t="s">
+        <v>133</v>
+      </c>
+      <c r="U71" t="s">
+        <v>137</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>1</v>
+      </c>
+      <c r="AF71">
+        <v>1</v>
+      </c>
+      <c r="AG71">
+        <v>0</v>
+      </c>
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AK71">
+        <v>0</v>
+      </c>
+      <c r="AL71">
+        <v>0</v>
+      </c>
+      <c r="AM71">
+        <v>0</v>
+      </c>
+      <c r="AN71">
+        <v>0</v>
+      </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
+      <c r="AP71">
+        <v>0</v>
+      </c>
+      <c r="AQ71">
         <v>0</v>
       </c>
     </row>
@@ -6873,16 +6904,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7031,21 +7060,21 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49">
       <c r="A2" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -7141,21 +7170,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -7251,21 +7280,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49">
       <c r="A4" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -7361,21 +7390,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -7471,21 +7500,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -7581,12 +7610,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49">
       <c r="A7" t="s">
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -7691,21 +7720,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49">
       <c r="A8" t="s">
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8">
         <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -7801,21 +7830,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -7911,21 +7940,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -8021,12 +8050,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -8131,12 +8160,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12">
         <v>30</v>
@@ -8241,12 +8270,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13">
         <v>40</v>
@@ -8351,21 +8380,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14">
         <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -8461,21 +8490,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15">
         <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -8571,21 +8600,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -8681,12 +8710,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E17">
         <v>20</v>
@@ -8791,21 +8820,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E18">
         <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -8901,21 +8930,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -9011,21 +9040,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -9121,21 +9150,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -9231,12 +9260,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -9341,12 +9370,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23">
         <v>30</v>
@@ -9451,12 +9480,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24">
         <v>40</v>
@@ -9561,21 +9590,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -9671,12 +9700,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E26">
         <v>20</v>
@@ -9781,12 +9810,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E27">
         <v>30</v>
@@ -9891,12 +9920,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28">
         <v>40</v>
@@ -10001,21 +10030,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E29">
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -10111,12 +10140,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E30">
         <v>20</v>
@@ -10221,12 +10250,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -10331,12 +10360,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32">
         <v>40</v>
@@ -10441,21 +10470,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -10551,21 +10580,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -10661,21 +10690,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E35">
         <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H35" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -10771,21 +10800,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E36">
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -10881,12 +10910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -10991,12 +11020,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E38">
         <v>30</v>
@@ -11101,12 +11130,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E39">
         <v>40</v>
@@ -11211,21 +11240,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E40">
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -11321,12 +11350,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E41">
         <v>20</v>
@@ -11431,12 +11460,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E42">
         <v>30</v>
@@ -11541,12 +11570,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E43">
         <v>40</v>
@@ -11651,21 +11680,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E44">
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -11761,12 +11790,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E45">
         <v>20</v>
@@ -11871,21 +11900,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E46">
         <v>30</v>
       </c>
       <c r="G46" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -11981,21 +12010,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E47">
         <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -12091,12 +12120,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E48">
         <v>20</v>
@@ -12201,21 +12230,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E49">
         <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -12311,21 +12340,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E50">
         <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -12421,12 +12450,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E51">
         <v>20</v>
@@ -12531,21 +12560,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E52">
         <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -12641,21 +12670,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E53">
         <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -12751,12 +12780,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E54">
         <v>20</v>
@@ -12861,21 +12890,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E55">
         <v>30</v>
       </c>
       <c r="G55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H55" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I55">
         <v>0</v>

</xml_diff>

<commit_message>
Made all 16ths thick bars -### part numbers for truncated thousandths instead of -316, -516, -1.5
</commit_message>
<xml_diff>
--- a/OpsAndMats/Model148.xlsx
+++ b/OpsAndMats/Model148.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="193">
   <si>
     <t>Item</t>
   </si>
@@ -317,13 +317,13 @@
     <t>2034701</t>
   </si>
   <si>
-    <t>9030240-3</t>
+    <t>9030240-312</t>
   </si>
   <si>
     <t>6960011</t>
   </si>
   <si>
-    <t>9816001</t>
+    <t>9816011</t>
   </si>
   <si>
     <t>3130003</t>
@@ -401,7 +401,7 @@
     <t>swivel pad with 1"-8 thd.</t>
   </si>
   <si>
-    <t>Nickel Plating, Electroless</t>
+    <t>Zinc Plating</t>
   </si>
   <si>
     <t>1"-8 heavy square nut, unplated</t>
@@ -548,25 +548,25 @@
     <t>FIN010</t>
   </si>
   <si>
+    <t>FAB040</t>
+  </si>
+  <si>
     <t>FAB020</t>
   </si>
   <si>
     <t>FAB030</t>
   </si>
   <si>
-    <t>FAB040</t>
-  </si>
-  <si>
     <t>Finishing, Surface Prep</t>
   </si>
   <si>
+    <t>Fabrication, Drill</t>
+  </si>
+  <si>
     <t>Fabrication, Layout</t>
   </si>
   <si>
     <t>Fabrication, Check</t>
-  </si>
-  <si>
-    <t>Fabrication, Drill</t>
   </si>
   <si>
     <t>Mch Hours/Pc</t>
@@ -4250,7 +4250,7 @@
         <v>68</v>
       </c>
       <c r="E40">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G40" t="s">
         <v>74</v>
@@ -4333,7 +4333,7 @@
         <v>68</v>
       </c>
       <c r="E41">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
         <v>75</v>
@@ -6905,7 +6905,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW55"/>
+  <dimension ref="A1:AW53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8171,10 +8171,10 @@
         <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -8281,10 +8281,10 @@
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>183</v>
+        <v>80</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -8382,13 +8382,13 @@
     </row>
     <row r="14" spans="1:49">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
         <v>74</v>
@@ -8492,19 +8492,19 @@
     </row>
     <row r="15" spans="1:49">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -8608,13 +8608,13 @@
         <v>69</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -8712,19 +8712,19 @@
     </row>
     <row r="17" spans="1:49">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -8822,19 +8822,19 @@
     </row>
     <row r="18" spans="1:49">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
         <v>69</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -8932,7 +8932,7 @@
     </row>
     <row r="19" spans="1:49">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>69</v>
@@ -8941,10 +8941,10 @@
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -9042,19 +9042,19 @@
     </row>
     <row r="20" spans="1:49">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
         <v>69</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -9158,13 +9158,13 @@
         <v>69</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -9268,7 +9268,7 @@
         <v>69</v>
       </c>
       <c r="E22">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
         <v>177</v>
@@ -9372,19 +9372,19 @@
     </row>
     <row r="23" spans="1:49">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>69</v>
       </c>
       <c r="E23">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -9482,19 +9482,19 @@
     </row>
     <row r="24" spans="1:49">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
       </c>
       <c r="E24">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -9598,13 +9598,13 @@
         <v>69</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -9708,7 +9708,7 @@
         <v>69</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
         <v>177</v>
@@ -9812,19 +9812,19 @@
     </row>
     <row r="27" spans="1:49">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>69</v>
       </c>
       <c r="E27">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -9922,19 +9922,19 @@
     </row>
     <row r="28" spans="1:49">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
         <v>69</v>
       </c>
       <c r="E28">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -10038,13 +10038,13 @@
         <v>69</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -10148,7 +10148,7 @@
         <v>69</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
         <v>177</v>
@@ -10252,19 +10252,19 @@
     </row>
     <row r="31" spans="1:49">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
         <v>69</v>
       </c>
       <c r="E31">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="H31" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -10362,19 +10362,19 @@
     </row>
     <row r="32" spans="1:49">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>69</v>
       </c>
       <c r="E32">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>179</v>
+        <v>72</v>
       </c>
       <c r="H32" t="s">
-        <v>183</v>
+        <v>77</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -10472,19 +10472,19 @@
     </row>
     <row r="33" spans="1:49">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H33" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -10582,10 +10582,10 @@
     </row>
     <row r="34" spans="1:49">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E34">
         <v>10</v>
@@ -10692,19 +10692,19 @@
     </row>
     <row r="35" spans="1:49">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
         <v>70</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G35" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="H35" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -10808,13 +10808,13 @@
         <v>70</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -10918,7 +10918,7 @@
         <v>70</v>
       </c>
       <c r="E37">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
         <v>177</v>
@@ -11022,19 +11022,19 @@
     </row>
     <row r="38" spans="1:49">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
         <v>70</v>
       </c>
       <c r="E38">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="H38" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -11132,19 +11132,19 @@
     </row>
     <row r="39" spans="1:49">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
         <v>70</v>
       </c>
       <c r="E39">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -11248,13 +11248,13 @@
         <v>70</v>
       </c>
       <c r="E40">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="H40" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -11358,7 +11358,7 @@
         <v>70</v>
       </c>
       <c r="E41">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G41" t="s">
         <v>177</v>
@@ -11462,19 +11462,19 @@
     </row>
     <row r="42" spans="1:49">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
         <v>70</v>
       </c>
       <c r="E42">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="H42" t="s">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -11572,19 +11572,19 @@
     </row>
     <row r="43" spans="1:49">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
         <v>70</v>
       </c>
       <c r="E43">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H43" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -11688,13 +11688,13 @@
         <v>70</v>
       </c>
       <c r="E44">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -11792,19 +11792,19 @@
     </row>
     <row r="45" spans="1:49">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
       </c>
       <c r="E45">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="H45" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -11902,19 +11902,19 @@
     </row>
     <row r="46" spans="1:49">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
       <c r="E46">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H46" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -12018,13 +12018,13 @@
         <v>70</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -12122,19 +12122,19 @@
     </row>
     <row r="48" spans="1:49">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>70</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G48" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="H48" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -12232,19 +12232,19 @@
     </row>
     <row r="49" spans="1:49">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
       </c>
       <c r="E49">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H49" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -12348,13 +12348,13 @@
         <v>70</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -12452,19 +12452,19 @@
     </row>
     <row r="51" spans="1:49">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
         <v>70</v>
       </c>
       <c r="E51">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="H51" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -12562,19 +12562,19 @@
     </row>
     <row r="52" spans="1:49">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
         <v>70</v>
       </c>
       <c r="E52">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G52" t="s">
-        <v>73</v>
+        <v>176</v>
       </c>
       <c r="H52" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -12678,13 +12678,13 @@
         <v>70</v>
       </c>
       <c r="E53">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -12777,226 +12777,6 @@
         <v>0</v>
       </c>
       <c r="AW53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:49">
-      <c r="A54" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54">
-        <v>20</v>
-      </c>
-      <c r="G54" t="s">
-        <v>176</v>
-      </c>
-      <c r="H54" t="s">
-        <v>180</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-      <c r="K54" t="s">
-        <v>184</v>
-      </c>
-      <c r="L54">
-        <v>0.5</v>
-      </c>
-      <c r="M54" t="s">
-        <v>185</v>
-      </c>
-      <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="O54" t="s">
-        <v>186</v>
-      </c>
-      <c r="P54">
-        <v>0.5</v>
-      </c>
-      <c r="R54">
-        <v>100</v>
-      </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
-      <c r="T54">
-        <v>0</v>
-      </c>
-      <c r="V54">
-        <v>0</v>
-      </c>
-      <c r="W54">
-        <v>0</v>
-      </c>
-      <c r="X54">
-        <v>0</v>
-      </c>
-      <c r="Y54">
-        <v>0</v>
-      </c>
-      <c r="AA54">
-        <v>0</v>
-      </c>
-      <c r="AD54">
-        <v>1</v>
-      </c>
-      <c r="AE54" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG54" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH54" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI54" t="s">
-        <v>189</v>
-      </c>
-      <c r="AK54" t="s">
-        <v>190</v>
-      </c>
-      <c r="AL54">
-        <v>0</v>
-      </c>
-      <c r="AM54" t="s">
-        <v>191</v>
-      </c>
-      <c r="AN54" t="s">
-        <v>192</v>
-      </c>
-      <c r="AO54">
-        <v>0</v>
-      </c>
-      <c r="AQ54">
-        <v>100</v>
-      </c>
-      <c r="AS54">
-        <v>35</v>
-      </c>
-      <c r="AT54">
-        <v>35</v>
-      </c>
-      <c r="AU54">
-        <v>0</v>
-      </c>
-      <c r="AV54">
-        <v>0</v>
-      </c>
-      <c r="AW54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:49">
-      <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" t="s">
-        <v>70</v>
-      </c>
-      <c r="E55">
-        <v>30</v>
-      </c>
-      <c r="G55" t="s">
-        <v>73</v>
-      </c>
-      <c r="H55" t="s">
-        <v>78</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="K55" t="s">
-        <v>184</v>
-      </c>
-      <c r="L55">
-        <v>0.5</v>
-      </c>
-      <c r="M55" t="s">
-        <v>185</v>
-      </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="O55" t="s">
-        <v>186</v>
-      </c>
-      <c r="P55">
-        <v>0.5</v>
-      </c>
-      <c r="R55">
-        <v>100</v>
-      </c>
-      <c r="S55">
-        <v>0</v>
-      </c>
-      <c r="T55">
-        <v>0</v>
-      </c>
-      <c r="V55">
-        <v>0</v>
-      </c>
-      <c r="W55">
-        <v>0</v>
-      </c>
-      <c r="X55">
-        <v>0</v>
-      </c>
-      <c r="Y55">
-        <v>0</v>
-      </c>
-      <c r="AA55">
-        <v>0</v>
-      </c>
-      <c r="AD55">
-        <v>1</v>
-      </c>
-      <c r="AE55" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG55" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH55" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI55" t="s">
-        <v>189</v>
-      </c>
-      <c r="AK55" t="s">
-        <v>190</v>
-      </c>
-      <c r="AL55">
-        <v>0</v>
-      </c>
-      <c r="AM55" t="s">
-        <v>191</v>
-      </c>
-      <c r="AN55" t="s">
-        <v>192</v>
-      </c>
-      <c r="AO55">
-        <v>0</v>
-      </c>
-      <c r="AQ55">
-        <v>100</v>
-      </c>
-      <c r="AS55">
-        <v>35</v>
-      </c>
-      <c r="AT55">
-        <v>35</v>
-      </c>
-      <c r="AU55">
-        <v>0</v>
-      </c>
-      <c r="AV55">
-        <v>0</v>
-      </c>
-      <c r="AW55">
         <v>0</v>
       </c>
     </row>

</xml_diff>